<commit_message>
worked on enchantments and creating more item templates.
</commit_message>
<xml_diff>
--- a/Emission Radiuses.xlsx
+++ b/Emission Radiuses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles\Documents\Git Repositories\materials_and_crafting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35EF1B7B-3681-4F96-AD09-522D3AF36DA2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B4C718-0D1F-4690-8E6B-5EC4508F54D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{B6414544-9ABE-4A7A-9980-FA57EE50A789}"/>
   </bookViews>
@@ -104,16 +104,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -124,9 +121,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -135,6 +129,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -450,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B8C45F3-51FB-4085-8BA1-2B57C18841E4}">
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,579 +481,608 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="11">
         <v>5</v>
       </c>
-      <c r="B2" s="4">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6">
-        <v>2</v>
-      </c>
-      <c r="D3" s="6"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="11">
         <v>8</v>
       </c>
-      <c r="B4" s="4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6">
-        <v>3</v>
-      </c>
-      <c r="D5" s="6"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5">
+        <v>3</v>
+      </c>
+      <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="11">
         <v>10</v>
       </c>
-      <c r="B6" s="4">
-        <v>2</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+      <c r="B6" s="3">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8">
-        <v>1</v>
-      </c>
-      <c r="C7" s="8">
-        <v>1</v>
-      </c>
-      <c r="D7" s="8"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="6">
+        <v>1</v>
+      </c>
+      <c r="C7" s="6">
+        <v>1</v>
+      </c>
+      <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6">
+      <c r="A8" s="10"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5">
         <v>4</v>
       </c>
-      <c r="D8" s="6"/>
+      <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="A9" s="11">
         <v>12</v>
       </c>
-      <c r="B9" s="4">
-        <v>2</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+      <c r="B9" s="3">
+        <v>2</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="9">
-        <v>1</v>
-      </c>
-      <c r="C10" s="9">
-        <v>2</v>
-      </c>
-      <c r="D10" s="9"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="7">
+        <v>1</v>
+      </c>
+      <c r="C10" s="7">
+        <v>2</v>
+      </c>
+      <c r="D10" s="7"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6">
+      <c r="A11" s="10"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5">
         <v>5</v>
       </c>
-      <c r="D11" s="6"/>
+      <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="A12" s="11">
         <v>14</v>
       </c>
-      <c r="B12" s="4">
-        <v>2</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="B12" s="3">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="9">
-        <v>1</v>
-      </c>
-      <c r="C13" s="9">
-        <v>3</v>
-      </c>
-      <c r="D13" s="9"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="7">
+        <v>1</v>
+      </c>
+      <c r="C13" s="7">
+        <v>3</v>
+      </c>
+      <c r="D13" s="7"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6">
+      <c r="A14" s="10"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5">
         <v>6</v>
       </c>
-      <c r="D14" s="6"/>
+      <c r="D14" s="5"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+      <c r="A15" s="11">
         <v>15</v>
       </c>
-      <c r="B15" s="4">
-        <v>2</v>
-      </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
+      <c r="B15" s="3">
+        <v>2</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="9">
-        <v>1</v>
-      </c>
-      <c r="C16" s="9">
-        <v>3</v>
-      </c>
-      <c r="D16" s="9"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="7">
+        <v>1</v>
+      </c>
+      <c r="C16" s="7">
+        <v>3</v>
+      </c>
+      <c r="D16" s="7"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6">
+      <c r="A17" s="10"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5">
         <v>6</v>
       </c>
-      <c r="D17" s="6"/>
+      <c r="D17" s="5"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
+      <c r="A18" s="11">
         <v>20</v>
       </c>
-      <c r="B18" s="4">
-        <v>3</v>
-      </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
+      <c r="B18" s="3">
+        <v>3</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="8">
-        <v>2</v>
-      </c>
-      <c r="C19" s="8">
-        <v>2</v>
-      </c>
-      <c r="D19" s="8"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="6">
+        <v>2</v>
+      </c>
+      <c r="C19" s="6">
+        <v>2</v>
+      </c>
+      <c r="D19" s="6"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6">
+      <c r="A20" s="10"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5">
         <v>8</v>
       </c>
-      <c r="D20" s="6"/>
+      <c r="D20" s="5"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
+      <c r="A21" s="11">
         <v>25</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="3">
         <v>4</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="9">
-        <v>3</v>
-      </c>
-      <c r="C22" s="9">
-        <v>1</v>
-      </c>
-      <c r="D22" s="9"/>
+      <c r="A22" s="9"/>
+      <c r="B22" s="7">
+        <v>3</v>
+      </c>
+      <c r="C22" s="7">
+        <v>1</v>
+      </c>
+      <c r="D22" s="7"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="9">
-        <v>2</v>
-      </c>
-      <c r="C23" s="9">
+      <c r="A23" s="9"/>
+      <c r="B23" s="7">
+        <v>2</v>
+      </c>
+      <c r="C23" s="7">
         <v>4</v>
       </c>
-      <c r="D23" s="9"/>
+      <c r="D23" s="7"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="6">
-        <v>1</v>
-      </c>
-      <c r="C24" s="6">
+      <c r="A24" s="10"/>
+      <c r="B24" s="5">
+        <v>1</v>
+      </c>
+      <c r="C24" s="5">
         <v>7</v>
       </c>
-      <c r="D24" s="6"/>
+      <c r="D24" s="5"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
+      <c r="A25" s="11">
         <v>30</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="3">
         <v>4</v>
       </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="8">
-        <v>3</v>
-      </c>
-      <c r="C26" s="8">
-        <v>3</v>
-      </c>
-      <c r="D26" s="8"/>
+      <c r="A26" s="9"/>
+      <c r="B26" s="6">
+        <v>3</v>
+      </c>
+      <c r="C26" s="6">
+        <v>3</v>
+      </c>
+      <c r="D26" s="6"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="9">
-        <v>2</v>
-      </c>
-      <c r="C27" s="9">
+      <c r="A27" s="9"/>
+      <c r="B27" s="7">
+        <v>2</v>
+      </c>
+      <c r="C27" s="7">
         <v>6</v>
       </c>
-      <c r="D27" s="9"/>
+      <c r="D27" s="7"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="6">
-        <v>1</v>
-      </c>
-      <c r="C28" s="6">
+      <c r="A28" s="10"/>
+      <c r="B28" s="5">
+        <v>1</v>
+      </c>
+      <c r="C28" s="5">
         <v>9</v>
       </c>
-      <c r="D28" s="6"/>
+      <c r="D28" s="5"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="7">
+      <c r="A29" s="9">
         <v>35</v>
       </c>
-      <c r="B29" s="9">
+      <c r="B29" s="7">
         <v>5</v>
       </c>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
-      <c r="B30" s="9">
+      <c r="A30" s="9"/>
+      <c r="B30" s="7">
         <v>4</v>
       </c>
-      <c r="C30" s="9">
-        <v>2</v>
-      </c>
-      <c r="D30" s="9"/>
+      <c r="C30" s="7">
+        <v>2</v>
+      </c>
+      <c r="D30" s="7"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="9">
-        <v>3</v>
-      </c>
-      <c r="C31" s="9">
+      <c r="A31" s="9"/>
+      <c r="B31" s="7">
+        <v>3</v>
+      </c>
+      <c r="C31" s="7">
         <v>5</v>
       </c>
-      <c r="D31" s="9"/>
+      <c r="D31" s="7"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="6">
-        <v>2</v>
-      </c>
-      <c r="C32" s="6">
+      <c r="A32" s="10"/>
+      <c r="B32" s="5">
+        <v>2</v>
+      </c>
+      <c r="C32" s="5">
         <v>8</v>
       </c>
-      <c r="D32" s="6"/>
+      <c r="D32" s="5"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="7">
+      <c r="A33" s="9">
         <v>40</v>
       </c>
-      <c r="B33" s="9">
+      <c r="B33" s="7">
         <v>6</v>
       </c>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
-      <c r="B34" s="9">
+      <c r="A34" s="9"/>
+      <c r="B34" s="7">
         <v>5</v>
       </c>
-      <c r="C34" s="9">
-        <v>1</v>
-      </c>
-      <c r="D34" s="9"/>
+      <c r="C34" s="7">
+        <v>1</v>
+      </c>
+      <c r="D34" s="7"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
-      <c r="B35" s="8">
+      <c r="A35" s="9"/>
+      <c r="B35" s="6">
         <v>4</v>
       </c>
-      <c r="C35" s="8">
+      <c r="C35" s="6">
         <v>4</v>
       </c>
-      <c r="D35" s="8"/>
+      <c r="D35" s="6"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
-      <c r="B36" s="6">
-        <v>3</v>
-      </c>
-      <c r="C36" s="6">
+      <c r="A36" s="10"/>
+      <c r="B36" s="5">
+        <v>3</v>
+      </c>
+      <c r="C36" s="5">
         <v>7</v>
       </c>
-      <c r="D36" s="6"/>
+      <c r="D36" s="5"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="7">
+      <c r="A37" s="9">
         <v>45</v>
       </c>
-      <c r="B37" s="9">
+      <c r="B37" s="7">
         <v>6</v>
       </c>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="7"/>
-      <c r="B38" s="9">
+      <c r="A38" s="9"/>
+      <c r="B38" s="7">
         <v>5</v>
       </c>
-      <c r="C38" s="9">
-        <v>3</v>
-      </c>
-      <c r="D38" s="9"/>
+      <c r="C38" s="7">
+        <v>3</v>
+      </c>
+      <c r="D38" s="7"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
-      <c r="B39" s="9">
+      <c r="A39" s="9"/>
+      <c r="B39" s="7">
         <v>4</v>
       </c>
-      <c r="C39" s="9">
+      <c r="C39" s="7">
         <v>6</v>
       </c>
-      <c r="D39" s="9"/>
+      <c r="D39" s="7"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="5"/>
-      <c r="B40" s="6">
-        <v>3</v>
-      </c>
-      <c r="C40" s="6">
+      <c r="A40" s="10"/>
+      <c r="B40" s="5">
+        <v>3</v>
+      </c>
+      <c r="C40" s="5">
         <v>9</v>
       </c>
-      <c r="D40" s="6"/>
+      <c r="D40" s="5"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="7">
+      <c r="A41" s="9">
         <v>50</v>
       </c>
-      <c r="B41" s="9">
+      <c r="B41" s="7">
         <v>7</v>
       </c>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="7"/>
-      <c r="B42" s="9">
+      <c r="A42" s="9"/>
+      <c r="B42" s="7">
         <v>6</v>
       </c>
-      <c r="C42" s="9">
-        <v>2</v>
-      </c>
-      <c r="D42" s="9"/>
+      <c r="C42" s="7">
+        <v>2</v>
+      </c>
+      <c r="D42" s="7"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="7"/>
-      <c r="B43" s="8">
+      <c r="A43" s="9"/>
+      <c r="B43" s="6">
         <v>5</v>
       </c>
-      <c r="C43" s="8">
+      <c r="C43" s="6">
         <v>5</v>
       </c>
-      <c r="D43" s="8"/>
+      <c r="D43" s="6"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
-      <c r="B44" s="6">
+      <c r="A44" s="10"/>
+      <c r="B44" s="5">
         <v>4</v>
       </c>
-      <c r="C44" s="6">
+      <c r="C44" s="5">
         <v>8</v>
       </c>
-      <c r="D44" s="6"/>
+      <c r="D44" s="5"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="7">
+      <c r="A45" s="9">
         <v>55</v>
       </c>
-      <c r="B45" s="9">
+      <c r="B45" s="7">
         <v>8</v>
       </c>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="7"/>
-      <c r="B46" s="9">
+      <c r="A46" s="9"/>
+      <c r="B46" s="7">
         <v>7</v>
       </c>
-      <c r="C46" s="9">
-        <v>1</v>
-      </c>
-      <c r="D46" s="9"/>
+      <c r="C46" s="7">
+        <v>1</v>
+      </c>
+      <c r="D46" s="7"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="7"/>
-      <c r="B47" s="9">
+      <c r="A47" s="9"/>
+      <c r="B47" s="7">
         <v>6</v>
       </c>
-      <c r="C47" s="9">
+      <c r="C47" s="7">
         <v>4</v>
       </c>
-      <c r="D47" s="9"/>
+      <c r="D47" s="7"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
-      <c r="B48" s="6">
+      <c r="A48" s="10"/>
+      <c r="B48" s="5">
         <v>5</v>
       </c>
-      <c r="C48" s="6">
+      <c r="C48" s="5">
         <v>7</v>
       </c>
-      <c r="D48" s="6"/>
+      <c r="D48" s="5"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="7">
+      <c r="A49" s="9">
         <v>60</v>
       </c>
-      <c r="B49" s="9">
+      <c r="B49" s="7">
         <v>8</v>
       </c>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="7"/>
-      <c r="B50" s="9">
+      <c r="A50" s="9"/>
+      <c r="B50" s="7">
         <v>7</v>
       </c>
-      <c r="C50" s="9">
-        <v>3</v>
-      </c>
-      <c r="D50" s="9"/>
+      <c r="C50" s="7">
+        <v>3</v>
+      </c>
+      <c r="D50" s="7"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="7"/>
-      <c r="B51" s="8">
+      <c r="A51" s="9"/>
+      <c r="B51" s="6">
         <v>6</v>
       </c>
-      <c r="C51" s="8">
+      <c r="C51" s="6">
         <v>6</v>
       </c>
-      <c r="D51" s="8"/>
+      <c r="D51" s="6"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="5"/>
-      <c r="B52" s="6">
+      <c r="A52" s="10"/>
+      <c r="B52" s="5">
         <v>5</v>
       </c>
-      <c r="C52" s="6">
+      <c r="C52" s="5">
         <v>9</v>
       </c>
-      <c r="D52" s="6"/>
+      <c r="D52" s="5"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="7">
+      <c r="A53" s="9">
         <v>65</v>
       </c>
-      <c r="B53" s="9">
+      <c r="B53" s="7">
         <v>8</v>
       </c>
-      <c r="C53" s="9">
-        <v>2</v>
-      </c>
-      <c r="D53" s="9"/>
+      <c r="C53" s="7">
+        <v>2</v>
+      </c>
+      <c r="D53" s="7"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="7"/>
-      <c r="B54" s="9">
+      <c r="A54" s="9"/>
+      <c r="B54" s="7">
         <v>7</v>
       </c>
-      <c r="C54" s="9">
+      <c r="C54" s="7">
         <v>5</v>
       </c>
-      <c r="D54" s="9"/>
+      <c r="D54" s="7"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="5"/>
-      <c r="B55" s="6">
+      <c r="A55" s="10"/>
+      <c r="B55" s="5">
         <v>6</v>
       </c>
-      <c r="C55" s="6">
+      <c r="C55" s="5">
         <v>8</v>
       </c>
-      <c r="D55" s="6"/>
+      <c r="D55" s="5"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="7">
+      <c r="A56" s="9">
         <v>70</v>
       </c>
-      <c r="B56" s="9">
+      <c r="B56" s="7">
         <v>8</v>
       </c>
-      <c r="C56" s="9">
+      <c r="C56" s="7">
         <v>4</v>
       </c>
-      <c r="D56" s="9"/>
+      <c r="D56" s="7"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="5"/>
-      <c r="B57" s="10">
+      <c r="A57" s="10"/>
+      <c r="B57" s="8">
         <v>7</v>
       </c>
-      <c r="C57" s="10">
+      <c r="C57" s="8">
         <v>7</v>
       </c>
-      <c r="D57" s="10"/>
+      <c r="D57" s="8"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="6">
+      <c r="A58" s="9">
+        <v>75</v>
+      </c>
+      <c r="B58" s="7">
+        <v>8</v>
+      </c>
+      <c r="C58" s="7">
+        <v>6</v>
+      </c>
+      <c r="D58" s="7"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="10"/>
+      <c r="B59" s="8">
+        <v>7</v>
+      </c>
+      <c r="C59" s="8">
+        <v>9</v>
+      </c>
+      <c r="D59" s="8"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="4">
+        <v>80</v>
+      </c>
+      <c r="B60" s="8">
+        <v>8</v>
+      </c>
+      <c r="C60" s="8">
+        <v>8</v>
+      </c>
+      <c r="D60" s="8"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="5">
         <v>120</v>
       </c>
-      <c r="B58" s="6">
+      <c r="B61" s="5">
         <v>11</v>
       </c>
-      <c r="C58" s="6">
+      <c r="C61" s="5">
         <v>7</v>
       </c>
-      <c r="D58" s="6">
+      <c r="D61" s="5">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="A37:A40"/>
-    <mergeCell ref="A41:A44"/>
+  <mergeCells count="18">
     <mergeCell ref="A45:A48"/>
     <mergeCell ref="A49:A52"/>
+    <mergeCell ref="A58:A59"/>
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="A21:A24"/>
     <mergeCell ref="A25:A28"/>
@@ -1060,6 +1092,12 @@
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="A41:A44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>